<commit_message>
Segment disks is done either here or the essay
Test functions not working as of now.
</commit_message>
<xml_diff>
--- a/disk_tracks_by_color.xlsx
+++ b/disk_tracks_by_color.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,10 +512,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>857.9265235843037</v>
+        <v>858.25706352359</v>
       </c>
       <c r="D3" t="n">
-        <v>22.3651713942677</v>
+        <v>21.6104626205988</v>
       </c>
       <c r="E3" t="n">
         <v>860.993335712348</v>
@@ -524,7 +524,7 @@
         <v>41.60105849861216</v>
       </c>
       <c r="G3" t="n">
-        <v>54.70096206665039</v>
+        <v>54.75259017944336</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -540,10 +540,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>850.7902161708248</v>
+        <v>850.9871798877329</v>
       </c>
       <c r="D4" t="n">
-        <v>37.76795708025037</v>
+        <v>37.48242997014471</v>
       </c>
       <c r="E4" t="n">
         <v>853.5645752661673</v>
@@ -552,7 +552,7 @@
         <v>57.20145543559171</v>
       </c>
       <c r="G4" t="n">
-        <v>55.33960342407227</v>
+        <v>55.52391815185547</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>843.7894800081642</v>
+        <v>843.8314662885181</v>
       </c>
       <c r="D5" t="n">
-        <v>52.65545440846379</v>
+        <v>52.73091409213418</v>
       </c>
       <c r="E5" t="n">
         <v>845.3929387753684</v>
@@ -580,7 +580,7 @@
         <v>72.0589763279532</v>
       </c>
       <c r="G5" t="n">
-        <v>55.75294494628906</v>
+        <v>55.68231201171875</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -596,10 +596,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>836.7557351931305</v>
+        <v>836.5930496921485</v>
       </c>
       <c r="D6" t="n">
-        <v>67.39010535322949</v>
+        <v>68.00067473902214</v>
       </c>
       <c r="E6" t="n">
         <v>837.9641783291877</v>
@@ -608,7 +608,7 @@
         <v>87.65937326493275</v>
       </c>
       <c r="G6" t="n">
-        <v>55.39266967773438</v>
+        <v>55.50335311889648</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -624,10 +624,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>828.6057719658405</v>
+        <v>829.0294434600368</v>
       </c>
       <c r="D7" t="n">
-        <v>84.2801918259519</v>
+        <v>83.48983183738081</v>
       </c>
       <c r="E7" t="n">
         <v>829.0496657937708</v>
@@ -636,7 +636,7 @@
         <v>104.0026462465304</v>
       </c>
       <c r="G7" t="n">
-        <v>55.17672729492188</v>
+        <v>55.2779655456543</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -652,10 +652,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>820.8990677847044</v>
+        <v>820.878029302972</v>
       </c>
       <c r="D8" t="n">
-        <v>100.9111909830949</v>
+        <v>101.0311420680581</v>
       </c>
       <c r="E8" t="n">
         <v>820.135153258354</v>
@@ -664,7 +664,7 @@
         <v>121.8316713173642</v>
       </c>
       <c r="G8" t="n">
-        <v>55.68236541748047</v>
+        <v>55.71365356445312</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -680,10 +680,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>813.8486372772622</v>
+        <v>813.7746398587553</v>
       </c>
       <c r="D9" t="n">
-        <v>116.4431675128889</v>
+        <v>116.7315511409884</v>
       </c>
       <c r="E9" t="n">
         <v>811.9635167675551</v>
@@ -692,7 +692,7 @@
         <v>138.1749442989618</v>
       </c>
       <c r="G9" t="n">
-        <v>56.40235137939453</v>
+        <v>56.43114471435547</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -708,10 +708,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>806.5924467911533</v>
+        <v>806.5271549512943</v>
       </c>
       <c r="D10" t="n">
-        <v>131.8697702677993</v>
+        <v>132.157213058623</v>
       </c>
       <c r="E10" t="n">
         <v>803.7918802767563</v>
@@ -720,7 +720,7 @@
         <v>150.8038370574691</v>
       </c>
       <c r="G10" t="n">
-        <v>56.4122200012207</v>
+        <v>56.42086791992188</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -848,10 +848,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>775.8524138037548</v>
+        <v>775.8497839935383</v>
       </c>
       <c r="D15" t="n">
-        <v>213.7956358327795</v>
+        <v>213.6443764037728</v>
       </c>
       <c r="E15" t="n">
         <v>768.8767061797068</v>
@@ -860,7 +860,7 @@
         <v>232.5202019654572</v>
       </c>
       <c r="G15" t="n">
-        <v>56.84878921508789</v>
+        <v>56.8713264465332</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>780.4449692729488</v>
+        <v>780.391284871287</v>
       </c>
       <c r="D16" t="n">
-        <v>232.0050312123474</v>
+        <v>231.4058878985301</v>
       </c>
       <c r="E16" t="n">
         <v>773.3339624474153</v>
@@ -888,7 +888,7 @@
         <v>250.349227036291</v>
       </c>
       <c r="G16" t="n">
-        <v>56.59192657470703</v>
+        <v>56.67901992797852</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -932,10 +932,10 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>790.2658595019641</v>
+        <v>790.2939712663477</v>
       </c>
       <c r="D18" t="n">
-        <v>269.2885081048385</v>
+        <v>269.2848807804018</v>
       </c>
       <c r="E18" t="n">
         <v>780.762722893596</v>
@@ -944,7 +944,7 @@
         <v>287.4930292671947</v>
       </c>
       <c r="G18" t="n">
-        <v>56.84763336181641</v>
+        <v>56.81094741821289</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -988,10 +988,10 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>799.3509469690126</v>
+        <v>799.3346240090478</v>
       </c>
       <c r="D20" t="n">
-        <v>303.9622610898537</v>
+        <v>303.7301803382437</v>
       </c>
       <c r="E20" t="n">
         <v>788.1914833397767</v>
@@ -1000,7 +1000,7 @@
         <v>320.17957523039</v>
       </c>
       <c r="G20" t="n">
-        <v>57.42971420288086</v>
+        <v>57.33015060424805</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1103,7 +1103,7 @@
         <v>823.1066574368263</v>
       </c>
       <c r="D24" t="n">
-        <v>392.9814276029613</v>
+        <v>393.3528656252703</v>
       </c>
       <c r="E24" t="n">
         <v>808.2491365444647</v>
@@ -1112,7 +1112,7 @@
         <v>407.0960724507047</v>
       </c>
       <c r="G24" t="n">
-        <v>58.21521759033203</v>
+        <v>58.17440795898438</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1128,10 +1128,10 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>827.8207282746467</v>
+        <v>827.7015706669041</v>
       </c>
       <c r="D25" t="n">
-        <v>410.4605065487729</v>
+        <v>410.0331623885846</v>
       </c>
       <c r="E25" t="n">
         <v>812.7063928121732</v>
@@ -1140,7 +1140,7 @@
         <v>424.9250975215385</v>
       </c>
       <c r="G25" t="n">
-        <v>57.70983505249024</v>
+        <v>57.68012619018555</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1184,10 +1184,10 @@
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>838.1277706612789</v>
+        <v>838.1695755754108</v>
       </c>
       <c r="D27" t="n">
-        <v>447.7866271741718</v>
+        <v>447.9413779029488</v>
       </c>
       <c r="E27" t="n">
         <v>821.6209053475901</v>
@@ -1196,7 +1196,7 @@
         <v>461.3260237078241</v>
       </c>
       <c r="G27" t="n">
-        <v>58.51176071166992</v>
+        <v>58.58638763427734</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1240,10 +1240,10 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>847.4676776699994</v>
+        <v>847.4041088092478</v>
       </c>
       <c r="D29" t="n">
-        <v>482.5802405610394</v>
+        <v>482.2014118651907</v>
       </c>
       <c r="E29" t="n">
         <v>829.0496657937708</v>
@@ -1252,7 +1252,7 @@
         <v>494.0125696710194</v>
       </c>
       <c r="G29" t="n">
-        <v>59.13900375366211</v>
+        <v>59.00302505493164</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1324,10 +1324,10 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>862.8505258238932</v>
+        <v>862.7883172098053</v>
       </c>
       <c r="D32" t="n">
-        <v>535.9850661919405</v>
+        <v>536.2593372609039</v>
       </c>
       <c r="E32" t="n">
         <v>842.4214345968961</v>
@@ -1336,7 +1336,7 @@
         <v>546.0138927942845</v>
       </c>
       <c r="G32" t="n">
-        <v>60.25373077392578</v>
+        <v>60.11376953125</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -1380,10 +1380,10 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>871.5509355344391</v>
+        <v>871.5051405634268</v>
       </c>
       <c r="D34" t="n">
-        <v>569.8386584510602</v>
+        <v>570.1917331434089</v>
       </c>
       <c r="E34" t="n">
         <v>850.593071087695</v>
@@ -1392,7 +1392,7 @@
         <v>577.2146866682436</v>
       </c>
       <c r="G34" t="n">
-        <v>60.23086547851562</v>
+        <v>60.44887542724609</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -1408,10 +1408,10 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>876.2403405660907</v>
+        <v>876.2538523496171</v>
       </c>
       <c r="D35" t="n">
-        <v>585.157711036425</v>
+        <v>585.2650798397488</v>
       </c>
       <c r="E35" t="n">
         <v>855.7932034000215</v>
@@ -1420,7 +1420,7 @@
         <v>592.0722075606052</v>
       </c>
       <c r="G35" t="n">
-        <v>59.97118377685547</v>
+        <v>59.97185897827149</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -1492,10 +1492,10 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>890.3369394747619</v>
+        <v>889.7363452311699</v>
       </c>
       <c r="D38" t="n">
-        <v>634.4161421038353</v>
+        <v>634.8381359604797</v>
       </c>
       <c r="E38" t="n">
         <v>867.6792201139107</v>
@@ -1504,7 +1504,7 @@
         <v>638.1305223269258</v>
       </c>
       <c r="G38" t="n">
-        <v>64.111328125</v>
+        <v>64.13108825683594</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -1548,10 +1548,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>898.8606078021339</v>
+        <v>898.8032053929245</v>
       </c>
       <c r="D40" t="n">
-        <v>665.3152786093348</v>
+        <v>665.5657000201273</v>
       </c>
       <c r="E40" t="n">
         <v>876.5937326493275</v>
@@ -1560,7 +1560,7 @@
         <v>667.8455641116487</v>
       </c>
       <c r="G40" t="n">
-        <v>61.13564300537109</v>
+        <v>61.2762565612793</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -1576,10 +1576,10 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>902.7742188199052</v>
+        <v>902.8059579087256</v>
       </c>
       <c r="D41" t="n">
-        <v>681.3707233968872</v>
+        <v>681.3479619360476</v>
       </c>
       <c r="E41" t="n">
         <v>880.308112872418</v>
@@ -1588,7 +1588,7 @@
         <v>681.9602089593922</v>
       </c>
       <c r="G41" t="n">
-        <v>62.93815231323242</v>
+        <v>62.93911361694336</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -1626,25 +1626,25 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B43" t="n">
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>914.8350725716392</v>
+        <v>910.834587133611</v>
       </c>
       <c r="D43" t="n">
-        <v>723.7701106624422</v>
+        <v>709.8515227004976</v>
       </c>
       <c r="E43" t="n">
-        <v>892.1941295863071</v>
+        <v>888.4797493632168</v>
       </c>
       <c r="F43" t="n">
-        <v>722.0755153687682</v>
+        <v>709.4466226102609</v>
       </c>
       <c r="G43" t="n">
-        <v>63.25526428222656</v>
+        <v>65.73482513427734</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1654,27 +1654,55 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
+        <v>176</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>914.9709158717902</v>
+      </c>
+      <c r="D44" t="n">
+        <v>723.6714927793219</v>
+      </c>
+      <c r="E44" t="n">
+        <v>892.1941295863071</v>
+      </c>
+      <c r="F44" t="n">
+        <v>722.0755153687682</v>
+      </c>
+      <c r="G44" t="n">
+        <v>63.23577499389648</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
         <v>177</v>
       </c>
-      <c r="B44" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" t="n">
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
         <v>919.3091052148668</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D45" t="n">
         <v>738.0473503280567</v>
       </c>
-      <c r="E44" t="n">
+      <c r="E45" t="n">
         <v>896.6513858540155</v>
       </c>
-      <c r="F44" t="n">
+      <c r="F45" t="n">
         <v>736.9330362611296</v>
       </c>
-      <c r="G44" t="n">
+      <c r="G45" t="n">
         <v>62.94849014282227</v>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>green</t>
         </is>
@@ -1749,10 +1777,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>627.7707930528519</v>
+        <v>627.7302577022728</v>
       </c>
       <c r="D2" t="n">
-        <v>15.9718349592886</v>
+        <v>15.60039693697956</v>
       </c>
       <c r="E2" t="n">
         <v>612.1298607652932</v>
@@ -1761,7 +1789,7 @@
         <v>5.200132312326519</v>
       </c>
       <c r="G2" t="n">
-        <v>55.32867050170898</v>
+        <v>55.44376373291016</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -1777,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>633.4976582149299</v>
+        <v>633.444971327488</v>
       </c>
       <c r="D3" t="n">
         <v>31.57223189626816</v>
@@ -1789,7 +1817,7 @@
         <v>17.82902507083378</v>
       </c>
       <c r="G3" t="n">
-        <v>55.41948699951172</v>
+        <v>55.51166534423828</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1805,10 +1833,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>639.412282758158</v>
+        <v>639.328264855895</v>
       </c>
       <c r="D4" t="n">
-        <v>47.96083509793457</v>
+        <v>47.80178258908358</v>
       </c>
       <c r="E4" t="n">
         <v>622.5301253899462</v>
@@ -1817,7 +1845,7 @@
         <v>34.91517409704949</v>
       </c>
       <c r="G4" t="n">
-        <v>55.22876739501953</v>
+        <v>55.18511581420898</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1833,10 +1861,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>645.3283128896053</v>
+        <v>645.5225561131858</v>
       </c>
       <c r="D5" t="n">
-        <v>64.21195136806453</v>
+        <v>64.87613147549143</v>
       </c>
       <c r="E5" t="n">
         <v>626.9873816576546</v>
@@ -1845,7 +1873,7 @@
         <v>51.25844707864712</v>
       </c>
       <c r="G5" t="n">
-        <v>55.23124694824219</v>
+        <v>55.22041320800781</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1861,10 +1889,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>651.9689917603766</v>
+        <v>651.8737291523602</v>
       </c>
       <c r="D6" t="n">
-        <v>82.05499831492359</v>
+        <v>82.0878029302972</v>
       </c>
       <c r="E6" t="n">
         <v>634.4161421038353</v>
@@ -1873,7 +1901,7 @@
         <v>70.57322423871705</v>
       </c>
       <c r="G6" t="n">
-        <v>55.56473159790039</v>
+        <v>55.43023681640625</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1889,10 +1917,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>657.6924563057953</v>
+        <v>657.6662488867408</v>
       </c>
       <c r="D7" t="n">
-        <v>97.74311982632484</v>
+        <v>97.8441634826622</v>
       </c>
       <c r="E7" t="n">
         <v>640.35915046078</v>
@@ -1901,7 +1929,7 @@
         <v>86.17362117569661</v>
       </c>
       <c r="G7" t="n">
-        <v>55.84872055053711</v>
+        <v>55.8556022644043</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1973,10 +2001,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>675.6457625801385</v>
+        <v>675.7412972374877</v>
       </c>
       <c r="D10" t="n">
-        <v>147.8323328789968</v>
+        <v>148.1719297939857</v>
       </c>
       <c r="E10" t="n">
         <v>657.4452994869957</v>
@@ -1985,7 +2013,7 @@
         <v>137.4320682543437</v>
       </c>
       <c r="G10" t="n">
-        <v>55.61709213256836</v>
+        <v>55.56551361083984</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -2001,19 +2029,19 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>682.4148940775214</v>
+        <v>682.1042590810811</v>
       </c>
       <c r="D11" t="n">
-        <v>166.4452340959712</v>
+        <v>165.6552935167881</v>
       </c>
       <c r="E11" t="n">
-        <v>664.8740599331765</v>
+        <v>664.1311838885583</v>
       </c>
       <c r="F11" t="n">
         <v>156.0039693697956</v>
       </c>
       <c r="G11" t="n">
-        <v>55.9329719543457</v>
+        <v>55.89757919311523</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -2057,10 +2085,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>686.8290305259897</v>
+        <v>686.9555788072719</v>
       </c>
       <c r="D13" t="n">
-        <v>196.806608418354</v>
+        <v>196.6480263281409</v>
       </c>
       <c r="E13" t="n">
         <v>668.5884401562668</v>
@@ -2069,7 +2097,7 @@
         <v>187.9476392883728</v>
       </c>
       <c r="G13" t="n">
-        <v>57.02071762084961</v>
+        <v>57.03709030151367</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -2113,10 +2141,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>671.18850631243</v>
+        <v>671.2609621180513</v>
       </c>
       <c r="D15" t="n">
-        <v>227.6915076754397</v>
+        <v>227.510322819831</v>
       </c>
       <c r="E15" t="n">
         <v>652.9880432192872</v>
@@ -2125,7 +2153,7 @@
         <v>219.1484331623319</v>
       </c>
       <c r="G15" t="n">
-        <v>56.62606430053711</v>
+        <v>56.59653854370117</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -2141,10 +2169,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>664.1097373328269</v>
+        <v>664.1033895150628</v>
       </c>
       <c r="D16" t="n">
-        <v>242.0852751385804</v>
+        <v>242.1076058546433</v>
       </c>
       <c r="E16" t="n">
         <v>644.8164067284885</v>
@@ -2153,7 +2181,7 @@
         <v>235.4917061439295</v>
       </c>
       <c r="G16" t="n">
-        <v>56.93633270263672</v>
+        <v>56.93940734863281</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -2225,10 +2253,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>642.2163405723252</v>
+        <v>642.4219191847701</v>
       </c>
       <c r="D19" t="n">
-        <v>285.6358391556495</v>
+        <v>285.0608175493357</v>
       </c>
       <c r="E19" t="n">
         <v>622.5301253899462</v>
@@ -2237,7 +2265,7 @@
         <v>279.3213927763959</v>
       </c>
       <c r="G19" t="n">
-        <v>57.03079223632812</v>
+        <v>56.95405578613281</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -2281,10 +2309,10 @@
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>627.3469401924337</v>
+        <v>627.1992627463082</v>
       </c>
       <c r="D21" t="n">
-        <v>315.3457800153835</v>
+        <v>315.6439914256285</v>
       </c>
       <c r="E21" t="n">
         <v>606.1868524083486</v>
@@ -2293,7 +2321,7 @@
         <v>310.522186650355</v>
       </c>
       <c r="G21" t="n">
-        <v>57.64112854003906</v>
+        <v>57.6081428527832</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -2337,10 +2365,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>612.5718502478943</v>
+        <v>612.5558446788177</v>
       </c>
       <c r="D23" t="n">
-        <v>344.5577345715262</v>
+        <v>344.5799746044781</v>
       </c>
       <c r="E23" t="n">
         <v>591.3293315159871</v>
@@ -2349,7 +2377,7 @@
         <v>340.9801044796961</v>
       </c>
       <c r="G23" t="n">
-        <v>57.73726654052734</v>
+        <v>57.73277282714844</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -2421,10 +2449,10 @@
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>581.9805829039523</v>
+        <v>581.9907394123749</v>
       </c>
       <c r="D26" t="n">
-        <v>404.1008999802835</v>
+        <v>404.0579615272651</v>
       </c>
       <c r="E26" t="n">
         <v>559.3856615974099</v>
@@ -2433,7 +2461,7 @@
         <v>401.8959401383781</v>
       </c>
       <c r="G26" t="n">
-        <v>58.6318359375</v>
+        <v>58.62931060791016</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -2449,10 +2477,10 @@
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>574.5253883309398</v>
+        <v>574.2431824897714</v>
       </c>
       <c r="D27" t="n">
-        <v>418.470772443698</v>
+        <v>419.3535271869029</v>
       </c>
       <c r="E27" t="n">
         <v>551.9569011512291</v>
@@ -2461,7 +2489,7 @@
         <v>417.4963370753577</v>
       </c>
       <c r="G27" t="n">
-        <v>58.4069709777832</v>
+        <v>58.50009918212891</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -2477,19 +2505,19 @@
         <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>565.8795245116095</v>
+        <v>565.9747871196259</v>
       </c>
       <c r="D28" t="n">
-        <v>434.712434999515</v>
+        <v>434.5341066619001</v>
       </c>
       <c r="E28" t="n">
-        <v>543.7852646604304</v>
+        <v>543.0423886158122</v>
       </c>
       <c r="F28" t="n">
         <v>433.8396100569553</v>
       </c>
       <c r="G28" t="n">
-        <v>58.44195175170898</v>
+        <v>58.45481109619141</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -2505,10 +2533,10 @@
         <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>557.5458826431604</v>
+        <v>557.5898639519544</v>
       </c>
       <c r="D29" t="n">
-        <v>450.9344646618189</v>
+        <v>450.7554108593167</v>
       </c>
       <c r="E29" t="n">
         <v>534.8707521250134</v>
@@ -2517,7 +2545,7 @@
         <v>450.925759083171</v>
       </c>
       <c r="G29" t="n">
-        <v>59.0197639465332</v>
+        <v>58.99424362182617</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -2533,10 +2561,10 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>549.825575995387</v>
+        <v>549.8415815644636</v>
       </c>
       <c r="D30" t="n">
-        <v>465.9568474498244</v>
+        <v>465.7832799755325</v>
       </c>
       <c r="E30" t="n">
         <v>526.6991156342146</v>
@@ -2545,7 +2573,7 @@
         <v>466.5261560201506</v>
       </c>
       <c r="G30" t="n">
-        <v>59.67373657226562</v>
+        <v>59.69118118286133</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -2561,10 +2589,10 @@
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>542.0719433043522</v>
+        <v>542.0508594810644</v>
       </c>
       <c r="D31" t="n">
-        <v>481.5810940449747</v>
+        <v>481.5829530487485</v>
       </c>
       <c r="E31" t="n">
         <v>518.5274791434158</v>
@@ -2573,7 +2601,7 @@
         <v>481.3836769125121</v>
       </c>
       <c r="G31" t="n">
-        <v>59.90217208862305</v>
+        <v>59.87882614135742</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -2589,10 +2617,10 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>534.2146144759859</v>
+        <v>534.2000144951285</v>
       </c>
       <c r="D32" t="n">
-        <v>495.5254360104192</v>
+        <v>495.5464291505961</v>
       </c>
       <c r="E32" t="n">
         <v>511.0987186972351</v>
@@ -2601,7 +2629,7 @@
         <v>497.7269498941097</v>
       </c>
       <c r="G32" t="n">
-        <v>59.35886764526367</v>
+        <v>59.35115051269531</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -2645,10 +2673,10 @@
         <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>516.6930504927103</v>
+        <v>516.6702890318707</v>
       </c>
       <c r="D34" t="n">
-        <v>529.1703210897673</v>
+        <v>528.7848725268218</v>
       </c>
       <c r="E34" t="n">
         <v>493.2696936264013</v>
@@ -2657,7 +2685,7 @@
         <v>531.8992479465411</v>
       </c>
       <c r="G34" t="n">
-        <v>60.41969680786133</v>
+        <v>60.20981216430664</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -2701,10 +2729,10 @@
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>500.6667149837617</v>
+        <v>500.7255229811902</v>
       </c>
       <c r="D36" t="n">
-        <v>560.2866889874642</v>
+        <v>560.5580128553228</v>
       </c>
       <c r="E36" t="n">
         <v>476.9264206448037</v>
@@ -2713,7 +2741,7 @@
         <v>562.3571657758822</v>
       </c>
       <c r="G36" t="n">
-        <v>60.9712028503418</v>
+        <v>61.24988174438477</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -2729,10 +2757,10 @@
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>491.9772325880811</v>
+        <v>491.9203742775372</v>
       </c>
       <c r="D37" t="n">
-        <v>575.0827267306252</v>
+        <v>575.2321724974136</v>
       </c>
       <c r="E37" t="n">
         <v>468.0119081093868</v>
@@ -2741,7 +2769,7 @@
         <v>580.9290668913341</v>
       </c>
       <c r="G37" t="n">
-        <v>60.45634078979492</v>
+        <v>60.45911407470703</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -2785,10 +2813,10 @@
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>473.8749793040595</v>
+        <v>473.8906674822479</v>
       </c>
       <c r="D39" t="n">
-        <v>609.6802378901384</v>
+        <v>609.7395899862324</v>
       </c>
       <c r="E39" t="n">
         <v>450.182883038553</v>
@@ -2797,7 +2825,7 @@
         <v>615.8442409883835</v>
       </c>
       <c r="G39" t="n">
-        <v>62.62515640258789</v>
+        <v>62.6220817565918</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -2813,10 +2841,10 @@
         <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>465.8831220806503</v>
+        <v>466.1547179978416</v>
       </c>
       <c r="D40" t="n">
-        <v>626.2465006414767</v>
+        <v>626.6159436353456</v>
       </c>
       <c r="E40" t="n">
         <v>442.0112465477542</v>
@@ -2825,7 +2853,7 @@
         <v>632.9303900145992</v>
       </c>
       <c r="G40" t="n">
-        <v>63.92812728881836</v>
+        <v>63.95711517333984</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -2841,10 +2869,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>457.2325427395523</v>
+        <v>457.3392767610997</v>
       </c>
       <c r="D41" t="n">
-        <v>641.6225475620519</v>
+        <v>641.5229775062668</v>
       </c>
       <c r="E41" t="n">
         <v>433.8396100569553</v>
@@ -2853,7 +2881,7 @@
         <v>648.5307869515788</v>
       </c>
       <c r="G41" t="n">
-        <v>61.80940628051758</v>
+        <v>61.89397430419922</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -2897,10 +2925,10 @@
         <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>438.6169323646393</v>
+        <v>438.5884125262564</v>
       </c>
       <c r="D43" t="n">
-        <v>675.8614523594505</v>
+        <v>675.9574857739099</v>
       </c>
       <c r="E43" t="n">
         <v>414.5248328968854</v>
@@ -2909,7 +2937,7 @@
         <v>684.9317131378644</v>
       </c>
       <c r="G43" t="n">
-        <v>61.7876205444336</v>
+        <v>61.79985427856445</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -2925,10 +2953,10 @@
         <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>430.5768770677786</v>
+        <v>430.5161193834654</v>
       </c>
       <c r="D44" t="n">
-        <v>692.890017610235</v>
+        <v>692.8590946694129</v>
       </c>
       <c r="E44" t="n">
         <v>407.0960724507047</v>
@@ -2937,7 +2965,7 @@
         <v>701.274986119462</v>
       </c>
       <c r="G44" t="n">
-        <v>65.00740051269531</v>
+        <v>65.02391052246094</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -2953,10 +2981,10 @@
         <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>422.0417826684313</v>
+        <v>422.2350737193472</v>
       </c>
       <c r="D45" t="n">
-        <v>709.8622686491411</v>
+        <v>709.8313910498745</v>
       </c>
       <c r="E45" t="n">
         <v>398.1815599152878</v>
@@ -2965,7 +2993,7 @@
         <v>718.3611351456777</v>
       </c>
       <c r="G45" t="n">
-        <v>65.60164642333984</v>
+        <v>65.42839813232422</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -2981,10 +3009,10 @@
         <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>412.8770754299991</v>
+        <v>412.8737654964507</v>
       </c>
       <c r="D46" t="n">
-        <v>725.588125670072</v>
+        <v>725.4808928914147</v>
       </c>
       <c r="E46" t="n">
         <v>390.009923424489</v>
@@ -2993,7 +3021,7 @@
         <v>735.4472841718934</v>
       </c>
       <c r="G46" t="n">
-        <v>62.81161880493164</v>
+        <v>62.73726654052734</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
@@ -3009,10 +3037,10 @@
         <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>403.2777240409499</v>
+        <v>403.2413601134729</v>
       </c>
       <c r="D47" t="n">
-        <v>742.8799893333991</v>
+        <v>742.8314738690593</v>
       </c>
       <c r="E47" t="n">
         <v>380.352534844454</v>
@@ -3021,7 +3049,7 @@
         <v>754.0191852873453</v>
       </c>
       <c r="G47" t="n">
-        <v>62.11557769775391</v>
+        <v>62.04449844360352</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>

</xml_diff>